<commit_message>
fixed: a wrong datum
</commit_message>
<xml_diff>
--- a/data/smusl-stats.xlsx
+++ b/data/smusl-stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkgg3\smusl-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A3036D-3313-47D6-ABB2-3A36BC5BC66D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E12600-A641-4F66-80C6-64E0EEC64515}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8856" firstSheet="2" activeTab="3" xr2:uid="{DD9839B4-1DB4-4A06-B897-55FB0E07904A}"/>
   </bookViews>
@@ -3018,8 +3018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A538BE0-DDA8-4A75-9787-8F265BA42424}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4503,7 +4503,7 @@
         <v>13</v>
       </c>
       <c r="G40" s="18" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="H40" s="5">
         <v>6</v>

</xml_diff>

<commit_message>
input: Week 4 mathces
</commit_message>
<xml_diff>
--- a/data/smusl-stats.xlsx
+++ b/data/smusl-stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkgg3\smusl-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E12600-A641-4F66-80C6-64E0EEC64515}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C79A6B6-039B-4259-BC2A-7BA860398806}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8856" firstSheet="2" activeTab="3" xr2:uid="{DD9839B4-1DB4-4A06-B897-55FB0E07904A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8856" firstSheet="1" activeTab="1" xr2:uid="{DD9839B4-1DB4-4A06-B897-55FB0E07904A}"/>
   </bookViews>
   <sheets>
     <sheet name="2024-Table" sheetId="9" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1469" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497" uniqueCount="91">
   <si>
     <t>June</t>
   </si>
@@ -1263,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149181A1-9221-47EA-8488-A0CD6122034E}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1767,62 +1767,150 @@
       <c r="M13" s="20"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
+      <c r="A14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="5">
+        <v>9</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="16">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
+      <c r="I14" s="5">
+        <v>1</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K14" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L14" s="19"/>
       <c r="M14" s="20"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
+      <c r="A15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="5">
+        <v>9</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1</v>
+      </c>
+      <c r="I15" s="5">
+        <v>1</v>
+      </c>
+      <c r="J15" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="L15" s="19"/>
       <c r="M15" s="20"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="15"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
+      <c r="A16" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="5">
+        <v>11</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="16">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H16" s="5">
+        <v>0</v>
+      </c>
+      <c r="I16" s="5">
+        <v>1</v>
+      </c>
+      <c r="J16" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="K16" s="19" t="s">
+        <v>77</v>
+      </c>
       <c r="L16" s="19"/>
       <c r="M16" s="20"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="15"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
+      <c r="A17" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="5">
+        <v>11</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="16">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="H17" s="5">
+        <v>4</v>
+      </c>
+      <c r="I17" s="5">
+        <v>5</v>
+      </c>
+      <c r="J17" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="K17" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="L17" s="19"/>
       <c r="M17" s="20"/>
     </row>
@@ -3018,7 +3106,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A538BE0-DDA8-4A75-9787-8F265BA42424}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update data, add champion page, update css
</commit_message>
<xml_diff>
--- a/data/smusl-stats.xlsx
+++ b/data/smusl-stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kkgg3\smusl-stats\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BB2F761-443A-40E8-BF89-BABC27BE124C}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D58AE3F-EA20-4D98-A71C-777BCFA734B6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8856" activeTab="1" xr2:uid="{DD9839B4-1DB4-4A06-B897-55FB0E07904A}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1719" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1829" uniqueCount="93">
   <si>
     <t>June</t>
   </si>
@@ -305,6 +305,12 @@
   </si>
   <si>
     <t>Playoff</t>
+  </si>
+  <si>
+    <t>Eric Wiberg</t>
+  </si>
+  <si>
+    <t>Nick Benson</t>
   </si>
 </sst>
 </file>
@@ -1263,8 +1269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{149181A1-9221-47EA-8488-A0CD6122034E}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1576,7 +1582,7 @@
         <v>89</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="L8" s="19"/>
       <c r="M8" s="20"/>
@@ -1610,7 +1616,7 @@
         <v>1</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="K9" s="19" t="s">
         <v>89</v>
@@ -1872,7 +1878,7 @@
         <v>89</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="L16" s="19"/>
       <c r="M16" s="20"/>
@@ -1906,7 +1912,7 @@
         <v>5</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="K17" s="19" t="s">
         <v>89</v>
@@ -2012,7 +2018,7 @@
         <v>89</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="L20" s="19"/>
       <c r="M20" s="20"/>
@@ -2046,7 +2052,7 @@
         <v>1</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="K21" s="19" t="s">
         <v>89</v>
@@ -2160,7 +2166,7 @@
         <v>89</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="L24" s="19"/>
       <c r="M24" s="20"/>
@@ -2194,7 +2200,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="19" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="K25" s="19" t="s">
         <v>89</v>
@@ -2308,7 +2314,7 @@
         <v>89</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="L28" s="19"/>
       <c r="M28" s="20"/>
@@ -2342,7 +2348,7 @@
         <v>2</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="K29" s="19" t="s">
         <v>89</v>
@@ -2372,10 +2378,18 @@
       <c r="G30" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
+      <c r="H30" s="5">
+        <v>2</v>
+      </c>
+      <c r="I30" s="5">
+        <v>1</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K30" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L30" s="19"/>
       <c r="M30" s="20"/>
     </row>
@@ -2401,10 +2415,18 @@
       <c r="G31" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
+      <c r="H31" s="5">
+        <v>1</v>
+      </c>
+      <c r="I31" s="5">
+        <v>1</v>
+      </c>
+      <c r="J31" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K31" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="L31" s="19"/>
       <c r="M31" s="20"/>
     </row>
@@ -2430,10 +2452,18 @@
       <c r="G32" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
+      <c r="H32" s="5">
+        <v>2</v>
+      </c>
+      <c r="I32" s="5">
+        <v>3</v>
+      </c>
+      <c r="J32" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="K32" s="19" t="s">
+        <v>91</v>
+      </c>
       <c r="L32" s="19"/>
       <c r="M32" s="20"/>
     </row>
@@ -2459,10 +2489,18 @@
       <c r="G33" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
+      <c r="H33" s="5">
+        <v>1</v>
+      </c>
+      <c r="I33" s="5">
+        <v>6</v>
+      </c>
+      <c r="J33" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K33" s="19" t="s">
+        <v>89</v>
+      </c>
       <c r="L33" s="19"/>
       <c r="M33" s="20"/>
     </row>
@@ -2488,10 +2526,18 @@
       <c r="G34" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
+      <c r="H34" s="5">
+        <v>3</v>
+      </c>
+      <c r="I34" s="5">
+        <v>1</v>
+      </c>
+      <c r="J34" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K34" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L34" s="19"/>
       <c r="M34" s="20"/>
     </row>
@@ -2517,10 +2563,18 @@
       <c r="G35" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
+      <c r="H35" s="5">
+        <v>4</v>
+      </c>
+      <c r="I35" s="5">
+        <v>1</v>
+      </c>
+      <c r="J35" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K35" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="L35" s="19"/>
       <c r="M35" s="20"/>
     </row>
@@ -2546,10 +2600,18 @@
       <c r="G36" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
+      <c r="H36" s="5">
+        <v>1</v>
+      </c>
+      <c r="I36" s="5">
+        <v>2</v>
+      </c>
+      <c r="J36" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K36" s="19" t="s">
+        <v>91</v>
+      </c>
       <c r="L36" s="19"/>
       <c r="M36" s="20"/>
     </row>
@@ -2575,10 +2637,18 @@
       <c r="G37" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="19"/>
-      <c r="K37" s="19"/>
+      <c r="H37" s="5">
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <v>6</v>
+      </c>
+      <c r="J37" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K37" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L37" s="19"/>
       <c r="M37" s="20"/>
     </row>
@@ -2604,10 +2674,18 @@
       <c r="G38" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="19"/>
-      <c r="K38" s="19"/>
+      <c r="H38" s="5">
+        <v>7</v>
+      </c>
+      <c r="I38" s="5">
+        <v>1</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K38" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L38" s="19"/>
       <c r="M38" s="20"/>
     </row>
@@ -2633,10 +2711,18 @@
       <c r="G39" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="19"/>
-      <c r="K39" s="19"/>
+      <c r="H39" s="5">
+        <v>0</v>
+      </c>
+      <c r="I39" s="5">
+        <v>4</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K39" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="L39" s="19"/>
       <c r="M39" s="20"/>
     </row>
@@ -2662,10 +2748,18 @@
       <c r="G40" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="19"/>
-      <c r="K40" s="19"/>
+      <c r="H40" s="5">
+        <v>0</v>
+      </c>
+      <c r="I40" s="5">
+        <v>4</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K40" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L40" s="19"/>
       <c r="M40" s="20"/>
     </row>
@@ -2691,10 +2785,18 @@
       <c r="G41" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="19"/>
-      <c r="K41" s="19"/>
+      <c r="H41" s="5">
+        <v>0</v>
+      </c>
+      <c r="I41" s="5">
+        <v>0</v>
+      </c>
+      <c r="J41" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K41" s="19" t="s">
+        <v>91</v>
+      </c>
       <c r="L41" s="19"/>
       <c r="M41" s="20"/>
     </row>
@@ -2720,10 +2822,18 @@
       <c r="G42" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="19"/>
-      <c r="K42" s="19"/>
+      <c r="H42" s="5">
+        <v>0</v>
+      </c>
+      <c r="I42" s="5">
+        <v>1</v>
+      </c>
+      <c r="J42" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K42" s="19" t="s">
+        <v>92</v>
+      </c>
       <c r="L42" s="19"/>
       <c r="M42" s="20"/>
     </row>
@@ -2749,10 +2859,18 @@
       <c r="G43" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="19"/>
-      <c r="K43" s="19"/>
+      <c r="H43" s="5">
+        <v>3</v>
+      </c>
+      <c r="I43" s="5">
+        <v>4</v>
+      </c>
+      <c r="J43" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="K43" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="L43" s="19"/>
       <c r="M43" s="20"/>
     </row>
@@ -2778,10 +2896,18 @@
       <c r="G44" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="19"/>
-      <c r="K44" s="19"/>
+      <c r="H44" s="5">
+        <v>5</v>
+      </c>
+      <c r="I44" s="5">
+        <v>2</v>
+      </c>
+      <c r="J44" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K44" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L44" s="19"/>
       <c r="M44" s="20"/>
     </row>
@@ -2807,10 +2933,18 @@
       <c r="G45" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="19"/>
-      <c r="K45" s="19"/>
+      <c r="H45" s="5">
+        <v>2</v>
+      </c>
+      <c r="I45" s="5">
+        <v>1</v>
+      </c>
+      <c r="J45" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K45" s="19" t="s">
+        <v>91</v>
+      </c>
       <c r="L45" s="19"/>
       <c r="M45" s="20"/>
     </row>
@@ -2836,10 +2970,18 @@
       <c r="G46" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="19"/>
-      <c r="K46" s="19"/>
+      <c r="H46" s="5">
+        <v>1</v>
+      </c>
+      <c r="I46" s="5">
+        <v>0</v>
+      </c>
+      <c r="J46" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K46" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L46" s="19"/>
       <c r="M46" s="20"/>
     </row>
@@ -2865,10 +3007,18 @@
       <c r="G47" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="19"/>
-      <c r="K47" s="19"/>
+      <c r="H47" s="5">
+        <v>2</v>
+      </c>
+      <c r="I47" s="5">
+        <v>1</v>
+      </c>
+      <c r="J47" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K47" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="L47" s="19"/>
       <c r="M47" s="20"/>
     </row>
@@ -2894,10 +3044,18 @@
       <c r="G48" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="19"/>
-      <c r="K48" s="19"/>
+      <c r="H48" s="5">
+        <v>0</v>
+      </c>
+      <c r="I48" s="5">
+        <v>7</v>
+      </c>
+      <c r="J48" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K48" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L48" s="19"/>
       <c r="M48" s="20"/>
     </row>
@@ -2923,10 +3081,18 @@
       <c r="G49" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
-      <c r="J49" s="19"/>
-      <c r="K49" s="19"/>
+      <c r="H49" s="5">
+        <v>3</v>
+      </c>
+      <c r="I49" s="5">
+        <v>3</v>
+      </c>
+      <c r="J49" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K49" s="19" t="s">
+        <v>91</v>
+      </c>
       <c r="L49" s="19"/>
       <c r="M49" s="20"/>
     </row>
@@ -2952,10 +3118,18 @@
       <c r="G50" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="19"/>
-      <c r="K50" s="19"/>
+      <c r="H50" s="5">
+        <v>4</v>
+      </c>
+      <c r="I50" s="5">
+        <v>1</v>
+      </c>
+      <c r="J50" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="K50" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L50" s="19"/>
       <c r="M50" s="20"/>
     </row>
@@ -2981,10 +3155,18 @@
       <c r="G51" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="19"/>
-      <c r="K51" s="19"/>
+      <c r="H51" s="5">
+        <v>0</v>
+      </c>
+      <c r="I51" s="5">
+        <v>1</v>
+      </c>
+      <c r="J51" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K51" s="19" t="s">
+        <v>92</v>
+      </c>
       <c r="L51" s="19"/>
       <c r="M51" s="20"/>
     </row>
@@ -3010,10 +3192,18 @@
       <c r="G52" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="19"/>
-      <c r="K52" s="19"/>
+      <c r="H52" s="5">
+        <v>1</v>
+      </c>
+      <c r="I52" s="5">
+        <v>2</v>
+      </c>
+      <c r="J52" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K52" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="L52" s="19"/>
       <c r="M52" s="20"/>
     </row>
@@ -3039,10 +3229,18 @@
       <c r="G53" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
-      <c r="J53" s="19"/>
-      <c r="K53" s="19"/>
+      <c r="H53" s="5">
+        <v>8</v>
+      </c>
+      <c r="I53" s="5">
+        <v>1</v>
+      </c>
+      <c r="J53" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K53" s="19" t="s">
+        <v>91</v>
+      </c>
       <c r="L53" s="19"/>
       <c r="M53" s="20"/>
     </row>
@@ -3068,10 +3266,18 @@
       <c r="G54" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
-      <c r="J54" s="19"/>
-      <c r="K54" s="19"/>
+      <c r="H54" s="5">
+        <v>0</v>
+      </c>
+      <c r="I54" s="5">
+        <v>1</v>
+      </c>
+      <c r="J54" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="K54" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="L54" s="19"/>
       <c r="M54" s="20"/>
     </row>
@@ -3097,10 +3303,18 @@
       <c r="G55" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="19"/>
-      <c r="K55" s="19"/>
+      <c r="H55" s="5">
+        <v>1</v>
+      </c>
+      <c r="I55" s="5">
+        <v>2</v>
+      </c>
+      <c r="J55" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K55" s="19" t="s">
+        <v>92</v>
+      </c>
       <c r="L55" s="19"/>
       <c r="M55" s="20"/>
     </row>
@@ -3126,10 +3340,18 @@
       <c r="G56" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
-      <c r="J56" s="19"/>
-      <c r="K56" s="19"/>
+      <c r="H56" s="5">
+        <v>0</v>
+      </c>
+      <c r="I56" s="5">
+        <v>2</v>
+      </c>
+      <c r="J56" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K56" s="19" t="s">
+        <v>91</v>
+      </c>
       <c r="L56" s="19"/>
       <c r="M56" s="20"/>
     </row>
@@ -3155,116 +3377,286 @@
       <c r="G57" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="19"/>
-      <c r="K57" s="19"/>
+      <c r="H57" s="5">
+        <v>2</v>
+      </c>
+      <c r="I57" s="5">
+        <v>0</v>
+      </c>
+      <c r="J57" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K57" s="19" t="s">
+        <v>81</v>
+      </c>
       <c r="L57" s="19"/>
       <c r="M57" s="20"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A58" s="15"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="16"/>
-      <c r="F58" s="17"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="19"/>
-      <c r="K58" s="19"/>
-      <c r="L58" s="19"/>
+      <c r="A58" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58" s="5">
+        <v>1</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" s="16">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="F58" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G58" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H58" s="5">
+        <v>7</v>
+      </c>
+      <c r="I58" s="5">
+        <v>2</v>
+      </c>
+      <c r="J58" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K58" s="19" t="s">
+        <v>92</v>
+      </c>
       <c r="M58" s="20"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A59" s="15"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="16"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
-      <c r="J59" s="19"/>
-      <c r="K59" s="19"/>
-      <c r="L59" s="19"/>
+      <c r="A59" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" s="5">
+        <v>1</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" s="16">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="F59" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G59" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="H59" s="5">
+        <v>3</v>
+      </c>
+      <c r="I59" s="5">
+        <v>2</v>
+      </c>
+      <c r="J59" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="K59" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="M59" s="20"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A60" s="15"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="17"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="19"/>
-      <c r="K60" s="19"/>
-      <c r="L60" s="19"/>
+      <c r="A60" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C60" s="5">
+        <v>3</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" s="16">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="G60" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="H60" s="5">
+        <v>1</v>
+      </c>
+      <c r="I60" s="5">
+        <v>0</v>
+      </c>
+      <c r="J60" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="K60" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="L60" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="M60" s="20"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A61" s="15"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="16"/>
-      <c r="F61" s="17"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="19"/>
-      <c r="K61" s="19"/>
-      <c r="L61" s="19"/>
+      <c r="A61" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" s="5">
+        <v>3</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" s="16">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H61" s="5">
+        <v>1</v>
+      </c>
+      <c r="I61" s="5">
+        <v>2</v>
+      </c>
+      <c r="J61" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K61" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="L61" s="19" t="s">
+        <v>8</v>
+      </c>
       <c r="M61" s="20"/>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A62" s="15"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="16"/>
-      <c r="F62" s="17"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
-      <c r="J62" s="19"/>
-      <c r="K62" s="19"/>
-      <c r="L62" s="19"/>
+      <c r="A62" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C62" s="5">
+        <v>8</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62" s="16">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="G62" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H62" s="5">
+        <v>4</v>
+      </c>
+      <c r="I62" s="5">
+        <v>3</v>
+      </c>
+      <c r="J62" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="K62" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="L62" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="M62" s="20"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A63" s="15"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="16"/>
-      <c r="F63" s="17"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="19"/>
-      <c r="K63" s="19"/>
-      <c r="L63" s="19"/>
+      <c r="A63" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C63" s="5">
+        <v>8</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E63" s="16">
+        <v>0.88194444444444453</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="G63" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H63" s="5">
+        <v>0</v>
+      </c>
+      <c r="I63" s="5">
+        <v>4</v>
+      </c>
+      <c r="J63" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K63" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="L63" s="19" t="s">
+        <v>82</v>
+      </c>
       <c r="M63" s="20"/>
     </row>
     <row r="64" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="36"/>
-      <c r="B64" s="30"/>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="38"/>
-      <c r="G64" s="39"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="30"/>
-      <c r="J64" s="40"/>
-      <c r="K64" s="40"/>
-      <c r="L64" s="40"/>
+      <c r="A64" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C64" s="30">
+        <v>15</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E64" s="37">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="F64" s="38" t="s">
+        <v>84</v>
+      </c>
+      <c r="G64" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="H64" s="30">
+        <v>2</v>
+      </c>
+      <c r="I64" s="30">
+        <v>0</v>
+      </c>
+      <c r="J64" s="40" t="s">
+        <v>82</v>
+      </c>
+      <c r="K64" s="40" t="s">
+        <v>81</v>
+      </c>
+      <c r="L64" s="40" t="s">
+        <v>91</v>
+      </c>
       <c r="M64" s="41"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.3">
@@ -3754,8 +4146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A538BE0-DDA8-4A75-9787-8F265BA42424}">
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58:A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>